<commit_message>
Genrate Pdf Issue Resolve
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="107">
   <si>
     <t>SR</t>
   </si>
@@ -42,138 +42,12 @@
     <t>exam2d</t>
   </si>
   <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>SHYAM</t>
-  </si>
-  <si>
-    <t>PAYAL</t>
-  </si>
-  <si>
-    <t>ROHIT</t>
-  </si>
-  <si>
-    <t>KAPOOR</t>
-  </si>
-  <si>
-    <t>NAINA</t>
-  </si>
-  <si>
-    <t>ANJALI</t>
-  </si>
-  <si>
-    <t>SONIA</t>
-  </si>
-  <si>
-    <t>YALPA</t>
-  </si>
-  <si>
-    <t>KAMIN</t>
-  </si>
-  <si>
-    <t>SORIA</t>
-  </si>
-  <si>
-    <t>RAM LAL</t>
-  </si>
-  <si>
-    <t>KRISHNA</t>
-  </si>
-  <si>
-    <t>RAM BHIARI</t>
-  </si>
-  <si>
-    <t>SALESH</t>
-  </si>
-  <si>
-    <t>KAMLESH</t>
-  </si>
-  <si>
-    <t>PANKAJ</t>
-  </si>
-  <si>
-    <t>NEHHAR</t>
-  </si>
-  <si>
-    <t>KUMAR</t>
-  </si>
-  <si>
-    <t>RAJA</t>
-  </si>
-  <si>
-    <t>OM PAL</t>
-  </si>
-  <si>
-    <t>DARAM</t>
-  </si>
-  <si>
-    <t>SANDEEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3rd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5th </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6th </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7th </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8th </t>
-  </si>
-  <si>
     <t xml:space="preserve">9th </t>
   </si>
   <si>
     <t xml:space="preserve">10th </t>
   </si>
   <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>HPS001</t>
-  </si>
-  <si>
-    <t>HPS002</t>
-  </si>
-  <si>
-    <t>HPS003</t>
-  </si>
-  <si>
-    <t>HPS004</t>
-  </si>
-  <si>
-    <t>HPS005</t>
-  </si>
-  <si>
-    <t>HPS006</t>
-  </si>
-  <si>
-    <t>HPS007</t>
-  </si>
-  <si>
-    <t>HPS008</t>
-  </si>
-  <si>
-    <t>HPS009</t>
-  </si>
-  <si>
-    <t>HPS010</t>
-  </si>
-  <si>
-    <t>HPS011</t>
-  </si>
-  <si>
-    <t>HPS012</t>
-  </si>
-  <si>
     <t>UDAI001</t>
   </si>
   <si>
@@ -280,6 +154,189 @@
   </si>
   <si>
     <t>img5.jpg</t>
+  </si>
+  <si>
+    <t>Aarav Sharma</t>
+  </si>
+  <si>
+    <t>Mr. Rajesh Sharma</t>
+  </si>
+  <si>
+    <t>Priya Mehta</t>
+  </si>
+  <si>
+    <t>Mr. Suresh Mehta</t>
+  </si>
+  <si>
+    <t>Rohan Gupta</t>
+  </si>
+  <si>
+    <t>Mr. Anil Gupta</t>
+  </si>
+  <si>
+    <t>Neha Verma</t>
+  </si>
+  <si>
+    <t>Mr. Sanjay Verma</t>
+  </si>
+  <si>
+    <t>Karan Yadav</t>
+  </si>
+  <si>
+    <t>Mr. Mahesh Yadav</t>
+  </si>
+  <si>
+    <t>Ananya Singh</t>
+  </si>
+  <si>
+    <t>Mr. Rakesh Singh</t>
+  </si>
+  <si>
+    <t>Aditya Kumar</t>
+  </si>
+  <si>
+    <t>Mr. Manoj Kumar</t>
+  </si>
+  <si>
+    <t>Pooja Patel</t>
+  </si>
+  <si>
+    <t>Mr. Harish Patel</t>
+  </si>
+  <si>
+    <t>Vikas Chaudhary</t>
+  </si>
+  <si>
+    <t>Mr. Om Prakash Chaudhary</t>
+  </si>
+  <si>
+    <t>Simran Kaur</t>
+  </si>
+  <si>
+    <t>Mr. Gurpreet Singh</t>
+  </si>
+  <si>
+    <t>Rahul Nair</t>
+  </si>
+  <si>
+    <t>Mr. Pradeep Nair</t>
+  </si>
+  <si>
+    <t>Sanya Rathi</t>
+  </si>
+  <si>
+    <t>Mr. Ajay Rathi</t>
+  </si>
+  <si>
+    <t>Amit Joshi</t>
+  </si>
+  <si>
+    <t>Mr. Dinesh Joshi</t>
+  </si>
+  <si>
+    <t>Ritika Saxena</t>
+  </si>
+  <si>
+    <t>Mr. Alok Saxena</t>
+  </si>
+  <si>
+    <t>Mohit Bansal</t>
+  </si>
+  <si>
+    <t>Mr. Vinod Bansal</t>
+  </si>
+  <si>
+    <t>Shreya Tiwari</t>
+  </si>
+  <si>
+    <t>Mr. Arun Tiwari</t>
+  </si>
+  <si>
+    <t>Deepak Chauhan</t>
+  </si>
+  <si>
+    <t>Mr. Kishan Chauhan</t>
+  </si>
+  <si>
+    <t>Ishita Pandey</t>
+  </si>
+  <si>
+    <t>Mr. Ravi Pandey</t>
+  </si>
+  <si>
+    <t>Arjun Malhotra</t>
+  </si>
+  <si>
+    <t>Mr. Vivek Malhotra</t>
+  </si>
+  <si>
+    <t>Kavya Agarwal</t>
+  </si>
+  <si>
+    <t>Mr. Pankaj Agarwal</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>HPS0901</t>
+  </si>
+  <si>
+    <t>HPS0902</t>
+  </si>
+  <si>
+    <t>HPS0903</t>
+  </si>
+  <si>
+    <t>HPS0904</t>
+  </si>
+  <si>
+    <t>HPS0905</t>
+  </si>
+  <si>
+    <t>HPS0906</t>
+  </si>
+  <si>
+    <t>HPS0907</t>
+  </si>
+  <si>
+    <t>HPS0908</t>
+  </si>
+  <si>
+    <t>HPS0909</t>
+  </si>
+  <si>
+    <t>HPS0910</t>
+  </si>
+  <si>
+    <t>HPS0911</t>
+  </si>
+  <si>
+    <t>HPS1001</t>
+  </si>
+  <si>
+    <t>HPS1002</t>
+  </si>
+  <si>
+    <t>HPS1003</t>
+  </si>
+  <si>
+    <t>HPS1004</t>
+  </si>
+  <si>
+    <t>HPS1005</t>
+  </si>
+  <si>
+    <t>HPS1006</t>
+  </si>
+  <si>
+    <t>HPS1007</t>
+  </si>
+  <si>
+    <t>HPS1008</t>
+  </si>
+  <si>
+    <t>HPS1009</t>
   </si>
 </sst>
 </file>
@@ -315,9 +372,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -627,7 +687,7 @@
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,13 +695,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -650,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -662,461 +722,672 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1">
         <v>46001</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1">
         <v>46001</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1">
         <v>46001</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1">
         <v>46001</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1">
         <v>46001</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1">
         <v>46001</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+      <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1">
         <v>46001</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1">
         <v>46001</v>
       </c>
       <c r="J9" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1">
         <v>46001</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="B11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1">
         <v>46001</v>
       </c>
       <c r="J11" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="I12" s="1">
         <v>46001</v>
       </c>
       <c r="J12" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="I13" s="1">
         <v>46001</v>
       </c>
       <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K13" t="s">
+      <c r="C17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L13" t="s">
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>